<commit_message>
corrigi o valor de indirect na planilha cinema H -> L
</commit_message>
<xml_diff>
--- a/data/tablenma_r.xlsx
+++ b/data/tablenma_r.xlsx
@@ -412,17 +412,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>desipramina</t>
+          <t>imipramina</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.66 (-2.97;  4.28)</t>
+          <t>-0.26 (-3.31;  2.80)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2.43 (-1.26;  6.13)</t>
+          <t>.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -432,12 +432,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>2.40 (-0.76;  5.57)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>3.92 ( 0.10;  7.73)</t>
+          <t>.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -447,12 +447,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>3.72 ( 0.40;  7.03)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.46 ( 1.29;  3.62)</t>
+          <t>2.03 ( 1.32;  2.74)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -464,17 +464,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0.13 (-1.25;  1.52)</t>
+          <t>0.00 (-1.16;  1.17)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>imipramina</t>
+          <t>desipramina</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3.16 (-0.59;  6.91)</t>
+          <t>.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -484,12 +484,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>1.72 (-1.40;  4.83)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>4.81 ( 0.89;  8.72)</t>
+          <t>.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -499,12 +499,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>2.67 (-0.52;  5.86)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2.32 ( 1.47;  3.17)</t>
+          <t>2.04 ( 1.05;  3.02)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -516,17 +516,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0.67 (-1.29;  2.62)</t>
+          <t>0.56 (-0.83;  1.94)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.53 (-1.29;  2.36)</t>
+          <t>0.55 (-0.98;  2.09)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>amitriptilina</t>
+          <t>mianserina</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2.11 (-1.56;  5.79)</t>
+          <t>.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2.58 ( 0.83;  4.34)</t>
+          <t>1.47 ( 0.27;  2.66)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -568,22 +568,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0.83 (-0.99;  2.65)</t>
+          <t>0.79 (-0.37;  1.95)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.70 (-0.95;  2.34)</t>
+          <t>0.79 (-0.54;  2.12)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.16 (-2.02;  2.34)</t>
+          <t>0.24 (-1.27;  1.74)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>mianserina</t>
+          <t>fluoxetina</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1.47 ( 0.05;  2.89)</t>
+          <t>1.23 ( 0.31;  2.15)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -620,27 +620,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1.07 (-0.51;  2.65)</t>
+          <t>0.85 (-0.68;  2.39)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.94 (-0.44;  2.31)</t>
+          <t>0.85 (-0.79;  2.50)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.40 (-1.58;  2.39)</t>
+          <t>0.30 (-1.54;  2.13)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.24 (-1.55;  2.03)</t>
+          <t>0.06 (-1.61;  1.73)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>fluoxetina</t>
+          <t>amitriptilina</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -655,12 +655,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>1.26 (-1.83;  4.34)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1.23 ( 0.14;  2.33)</t>
+          <t>1.34 (-0.13;  2.81)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -672,32 +672,32 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1.73 (-0.24;  3.70)</t>
+          <t>1.63 (-0.55;  3.81)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1.60 (-0.24;  3.44)</t>
+          <t>1.63 (-0.64;  3.90)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.06 (-1.18;  3.31)</t>
+          <t>1.08 (-1.31;  3.46)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.90 (-1.29;  3.09)</t>
+          <t>0.84 (-1.42;  3.10)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.66 (-1.33;  2.66)</t>
+          <t>0.78 (-1.71;  3.27)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>clomipramina</t>
+          <t>citalopram</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -712,7 +712,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1.54 (-0.21;  3.28)</t>
+          <t>0.39 (-1.67;  2.45)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -724,37 +724,37 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1.91 (-0.79;  4.61)</t>
+          <t>1.67 (-0.16;  3.49)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.78 (-0.81;  4.37)</t>
+          <t>1.66 (-0.27;  3.60)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.24 (-1.71;  4.20)</t>
+          <t>1.11 (-0.95;  3.18)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.08 (-1.75;  3.91)</t>
+          <t>0.88 (-1.04;  2.80)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.84 (-1.84;  3.52)</t>
+          <t>0.81 (-1.37;  3.00)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.18 (-2.78;  3.14)</t>
+          <t>0.04 (-2.63;  2.70)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>citalopram</t>
+          <t>fluvoxamina</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.39 (-2.06;  2.84)</t>
+          <t>0.35 (-1.33;  2.04)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -776,47 +776,47 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1.95 (-0.36;  4.25)</t>
+          <t>1.88 ( 0.32;  3.43)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1.81 (-0.36;  3.98)</t>
+          <t>1.87 ( 0.22;  3.53)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.28 (-1.32;  3.88)</t>
+          <t>1.32 (-0.52;  3.16)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.12 (-1.34;  3.57)</t>
+          <t>1.09 (-0.59;  2.76)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.88 (-1.40;  3.16)</t>
+          <t>1.02 (-0.86;  2.91)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.22 (-2.39;  2.82)</t>
+          <t>0.24 (-2.25;  2.74)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.04 (-3.13;  3.20)</t>
+          <t>0.21 (-1.98;  2.40)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>fluvoxamina</t>
+          <t>clomipramina</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.35 (-1.65;  2.36)</t>
+          <t>0.24 (-1.22;  1.71)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -828,42 +828,42 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2.30 ( 1.16;  3.44)</t>
+          <t>2.02 ( 1.32;  2.73)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2.17 ( 1.33;  3.00)</t>
+          <t>2.02 ( 1.06;  2.98)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.63 (-0.02;  3.29)</t>
+          <t>1.47 ( 0.27;  2.66)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.47 ( 0.05;  2.89)</t>
+          <t>1.23 ( 0.31;  2.15)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.23 ( 0.14;  2.33)</t>
+          <t>1.17 (-0.22;  2.56)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0.57 (-1.10;  2.24)</t>
+          <t>0.39 (-1.67;  2.45)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.39 (-2.06;  2.84)</t>
+          <t>0.35 (-1.33;  2.04)</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.35 (-1.65;  2.36)</t>
+          <t>0.15 (-1.26;  1.55)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -873,54 +873,54 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.36 (-1.64;  2.36)</t>
+          <t>0.36 (-1.33;  2.04)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2.66 ( 0.35;  4.96)</t>
+          <t>2.38 ( 0.55;  4.20)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2.52 ( 0.35;  4.69)</t>
+          <t>2.38 ( 0.44;  4.31)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.99 (-0.61;  4.59)</t>
+          <t>1.82 (-0.24;  3.89)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.83 (-0.62;  4.28)</t>
+          <t>1.59 (-0.33;  3.51)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.59 (-0.69;  3.87)</t>
+          <t>1.52 (-0.66;  3.71)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0.93 (-1.68;  3.53)</t>
+          <t>0.75 (-1.92;  3.41)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.75 (-2.42;  3.91)</t>
+          <t>0.71 (-1.67;  3.09)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.71 (-2.12;  3.54)</t>
+          <t>0.50 (-1.69;  2.69)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.36 (-1.64;  2.36)</t>
+          <t>0.36 (-1.33;  2.04)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">

</xml_diff>